<commit_message>
Updated 'Gate' names in ML_stable_batchExport.xlsx
</commit_message>
<xml_diff>
--- a/data/ML_stable_batchExport.xlsx
+++ b/data/ML_stable_batchExport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hortowe/projs/Coussens/multiplex/data/oldVersions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hortowe/projs/Coussens/multiplex/code/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D947D4D-C3D0-8249-8FE0-8291A43FE956}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F90E3C-12B9-B844-A9B4-CFBDF4AE7D4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28440" yWindow="-21120" windowWidth="35900" windowHeight="21140" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28440" yWindow="-21140" windowWidth="35900" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cohort" sheetId="1" r:id="rId1"/>
@@ -19,148 +19,6 @@
     <sheet name="Ratio" sheetId="6" r:id="rId4"/>
     <sheet name="PerPatient" sheetId="3" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Ratio!$C$10</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Ratio!$C$11</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Ratio!$C$3</definedName>
-    <definedName name="_xlchart.v1.100" hidden="1">Ratio!$E$5:$G$5</definedName>
-    <definedName name="_xlchart.v1.101" hidden="1">Ratio!$E$6:$G$6</definedName>
-    <definedName name="_xlchart.v1.102" hidden="1">Ratio!$E$7:$G$7</definedName>
-    <definedName name="_xlchart.v1.103" hidden="1">Ratio!$E$8:$G$8</definedName>
-    <definedName name="_xlchart.v1.104" hidden="1">Ratio!$E$9:$G$9</definedName>
-    <definedName name="_xlchart.v1.105" hidden="1">Ratio!$C$10</definedName>
-    <definedName name="_xlchart.v1.106" hidden="1">Ratio!$C$11</definedName>
-    <definedName name="_xlchart.v1.107" hidden="1">Ratio!$C$12</definedName>
-    <definedName name="_xlchart.v1.108" hidden="1">Ratio!$C$13</definedName>
-    <definedName name="_xlchart.v1.109" hidden="1">Ratio!$C$14</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Ratio!$C$4</definedName>
-    <definedName name="_xlchart.v1.110" hidden="1">Ratio!$C$15</definedName>
-    <definedName name="_xlchart.v1.111" hidden="1">Ratio!$C$16</definedName>
-    <definedName name="_xlchart.v1.112" hidden="1">Ratio!$C$17</definedName>
-    <definedName name="_xlchart.v1.113" hidden="1">Ratio!$C$18</definedName>
-    <definedName name="_xlchart.v1.114" hidden="1">Ratio!$C$2</definedName>
-    <definedName name="_xlchart.v1.115" hidden="1">Ratio!$C$3</definedName>
-    <definedName name="_xlchart.v1.116" hidden="1">Ratio!$C$4</definedName>
-    <definedName name="_xlchart.v1.117" hidden="1">Ratio!$C$5</definedName>
-    <definedName name="_xlchart.v1.118" hidden="1">Ratio!$C$6</definedName>
-    <definedName name="_xlchart.v1.119" hidden="1">Ratio!$C$7</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Ratio!$C$5</definedName>
-    <definedName name="_xlchart.v1.120" hidden="1">Ratio!$C$8</definedName>
-    <definedName name="_xlchart.v1.121" hidden="1">Ratio!$C$9</definedName>
-    <definedName name="_xlchart.v1.122" hidden="1">Ratio!$E$10:$G$10</definedName>
-    <definedName name="_xlchart.v1.123" hidden="1">Ratio!$E$11:$G$11</definedName>
-    <definedName name="_xlchart.v1.124" hidden="1">Ratio!$E$12:$G$12</definedName>
-    <definedName name="_xlchart.v1.125" hidden="1">Ratio!$E$13:$G$13</definedName>
-    <definedName name="_xlchart.v1.126" hidden="1">Ratio!$E$14:$G$14</definedName>
-    <definedName name="_xlchart.v1.127" hidden="1">Ratio!$E$15:$G$15</definedName>
-    <definedName name="_xlchart.v1.128" hidden="1">Ratio!$E$16:$G$16</definedName>
-    <definedName name="_xlchart.v1.129" hidden="1">Ratio!$E$17:$G$17</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Ratio!$C$6</definedName>
-    <definedName name="_xlchart.v1.130" hidden="1">Ratio!$E$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.131" hidden="1">Ratio!$E$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.132" hidden="1">Ratio!$E$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.133" hidden="1">Ratio!$E$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.134" hidden="1">Ratio!$E$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.135" hidden="1">Ratio!$E$5:$G$5</definedName>
-    <definedName name="_xlchart.v1.136" hidden="1">Ratio!$E$6:$G$6</definedName>
-    <definedName name="_xlchart.v1.137" hidden="1">Ratio!$E$7:$G$7</definedName>
-    <definedName name="_xlchart.v1.138" hidden="1">Ratio!$E$8:$G$8</definedName>
-    <definedName name="_xlchart.v1.139" hidden="1">Ratio!$E$9:$G$9</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Ratio!$C$7</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Ratio!$C$8</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Ratio!$C$9</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Ratio!$E$10:$G$10</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Ratio!$E$11:$G$11</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Ratio!$E$12:$G$12</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Ratio!$C$12</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Ratio!$E$13:$G$13</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Ratio!$E$14:$G$14</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Ratio!$E$15:$G$15</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Ratio!$E$16:$G$16</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Ratio!$E$17:$G$17</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Ratio!$E$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Ratio!$E$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Ratio!$E$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Ratio!$E$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Ratio!$E$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Ratio!$C$13</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Ratio!$E$5:$G$5</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Ratio!$E$6:$G$6</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Ratio!$E$7:$G$7</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Ratio!$E$8:$G$8</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Ratio!$E$9:$G$9</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Ratio!$C$10</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Ratio!$C$11</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Ratio!$C$12</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Ratio!$C$13</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Ratio!$C$14</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Ratio!$C$14</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Ratio!$C$15</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Ratio!$C$16</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Ratio!$C$17</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Ratio!$C$18</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Ratio!$C$2</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">Ratio!$C$3</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">Ratio!$C$4</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">Ratio!$C$5</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">Ratio!$C$6</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">Ratio!$C$7</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Ratio!$C$15</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">Ratio!$C$8</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">Ratio!$C$9</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">Ratio!$E$10:$G$10</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">Ratio!$E$11:$G$11</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">Ratio!$E$12:$G$12</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">Ratio!$E$13:$G$13</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">Ratio!$E$14:$G$14</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">Ratio!$E$15:$G$15</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">Ratio!$E$16:$G$16</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">Ratio!$E$17:$G$17</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Ratio!$C$16</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">Ratio!$E$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">Ratio!$E$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">Ratio!$E$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">Ratio!$E$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">Ratio!$E$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">Ratio!$E$5:$G$5</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">Ratio!$E$6:$G$6</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">Ratio!$E$7:$G$7</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">Ratio!$E$8:$G$8</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">Ratio!$E$9:$G$9</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Ratio!$C$17</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">Ratio!$C$10</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">Ratio!$C$11</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">Ratio!$C$12</definedName>
-    <definedName name="_xlchart.v1.73" hidden="1">Ratio!$C$13</definedName>
-    <definedName name="_xlchart.v1.74" hidden="1">Ratio!$C$14</definedName>
-    <definedName name="_xlchart.v1.75" hidden="1">Ratio!$C$15</definedName>
-    <definedName name="_xlchart.v1.76" hidden="1">Ratio!$C$16</definedName>
-    <definedName name="_xlchart.v1.77" hidden="1">Ratio!$C$17</definedName>
-    <definedName name="_xlchart.v1.78" hidden="1">Ratio!$C$18</definedName>
-    <definedName name="_xlchart.v1.79" hidden="1">Ratio!$C$2</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Ratio!$C$18</definedName>
-    <definedName name="_xlchart.v1.80" hidden="1">Ratio!$C$3</definedName>
-    <definedName name="_xlchart.v1.81" hidden="1">Ratio!$C$4</definedName>
-    <definedName name="_xlchart.v1.82" hidden="1">Ratio!$C$5</definedName>
-    <definedName name="_xlchart.v1.83" hidden="1">Ratio!$C$6</definedName>
-    <definedName name="_xlchart.v1.84" hidden="1">Ratio!$C$7</definedName>
-    <definedName name="_xlchart.v1.85" hidden="1">Ratio!$C$8</definedName>
-    <definedName name="_xlchart.v1.86" hidden="1">Ratio!$C$9</definedName>
-    <definedName name="_xlchart.v1.87" hidden="1">Ratio!$E$10:$G$10</definedName>
-    <definedName name="_xlchart.v1.88" hidden="1">Ratio!$E$11:$G$11</definedName>
-    <definedName name="_xlchart.v1.89" hidden="1">Ratio!$E$12:$G$12</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Ratio!$C$2</definedName>
-    <definedName name="_xlchart.v1.90" hidden="1">Ratio!$E$13:$G$13</definedName>
-    <definedName name="_xlchart.v1.91" hidden="1">Ratio!$E$14:$G$14</definedName>
-    <definedName name="_xlchart.v1.92" hidden="1">Ratio!$E$15:$G$15</definedName>
-    <definedName name="_xlchart.v1.93" hidden="1">Ratio!$E$16:$G$16</definedName>
-    <definedName name="_xlchart.v1.94" hidden="1">Ratio!$E$17:$G$17</definedName>
-    <definedName name="_xlchart.v1.95" hidden="1">Ratio!$E$18:$G$18</definedName>
-    <definedName name="_xlchart.v1.96" hidden="1">Ratio!$E$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.97" hidden="1">Ratio!$E$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.98" hidden="1">Ratio!$E$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.99" hidden="1">Ratio!$E$4:$G$4</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -174,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="221">
   <si>
     <t>syn80_2</t>
   </si>
@@ -341,55 +199,7 @@
     <t>CD45-</t>
   </si>
   <si>
-    <t>CD45+ C3/20/NKp46- CD66b- Tryptase- CD68-</t>
-  </si>
-  <si>
-    <t>CD45+ CD3/CD20/NKp46- CD66b- Tryptase-</t>
-  </si>
-  <si>
     <t>CD45+ PDL1+</t>
-  </si>
-  <si>
-    <t>CD45+ CD3/CD20/NKp46+ PDL1+</t>
-  </si>
-  <si>
-    <t>CD45+ CD3/CD20/NKp46- PDL1+</t>
-  </si>
-  <si>
-    <t>CD45+ CD3/CD20/NKp46- Tryptase+ PDL1+</t>
-  </si>
-  <si>
-    <t>CD45+ CD3/CD20/NKp46- CD66b+ PDL1+</t>
-  </si>
-  <si>
-    <t>CD45+ CD3/20/NKp46- CD66B- Tryptase- CD68+ CSF1R+ CD163+ PD-L1+</t>
-  </si>
-  <si>
-    <t>CD45+ CD3/20/NKp46- CD66b- Tryptase- CD68+ CSF1R- CD163+ PD-L1+</t>
-  </si>
-  <si>
-    <t>CD45+ CD3/20/NKp46- CD66b- Tryptase- CD68+ CSF1R+ CD163- PD-L1+</t>
-  </si>
-  <si>
-    <t>CD45+ CD3/20/NKp46- CD66B- Tryptase- CD68+ CD163- CSF1R- PD-L1+</t>
-  </si>
-  <si>
-    <t>CD45+ CD3/20/NKp46- CD66B- Tryptase- CD68+ PD-L1+</t>
-  </si>
-  <si>
-    <t>DC-sign+ DCs PD-L1+</t>
-  </si>
-  <si>
-    <t>mature DC PD-L1+</t>
-  </si>
-  <si>
-    <t>dual neg DCs PD-L1+</t>
-  </si>
-  <si>
-    <t>total DCs PD-L1+</t>
-  </si>
-  <si>
-    <t>other myeloid PD-L1+</t>
   </si>
   <si>
     <t>CD45- PDL1+</t>
@@ -437,37 +247,7 @@
     <t>NKp46+ PDL1+</t>
   </si>
   <si>
-    <t>CD45-pos PDL1+</t>
-  </si>
-  <si>
-    <t>Th17 PD-1+</t>
-  </si>
-  <si>
-    <t>Treg PD-1+</t>
-  </si>
-  <si>
-    <t>Th0 PD-1+</t>
-  </si>
-  <si>
-    <t>Th1 PD-1+</t>
-  </si>
-  <si>
-    <t>Th2 PD-1+</t>
-  </si>
-  <si>
-    <t>CD8+T PD1+</t>
-  </si>
-  <si>
-    <t>CD8+ T PDL1+</t>
-  </si>
-  <si>
     <t>CD45+ CD3+ PD1+</t>
-  </si>
-  <si>
-    <t>CD45+ CD3+ PD-L1+</t>
-  </si>
-  <si>
-    <t>CD45+ PD-1+</t>
   </si>
   <si>
     <t>PD1+</t>
@@ -647,28 +427,7 @@
     <t>Panel</t>
   </si>
   <si>
-    <t>CD45+ CD3/CD20/NKp46+</t>
-  </si>
-  <si>
-    <t>CD45+ CD3/CD20/NKp46-</t>
-  </si>
-  <si>
-    <t>CD45+ CD3/20/NKp46- CD66B- Tryptase- CD68+</t>
-  </si>
-  <si>
-    <t>CD45+ CD3/CD20/NKp46- CD66b- Tryptase- CD68- MHCII+CSF1R-</t>
-  </si>
-  <si>
     <t>CD45+ CD3+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD45+ CD3/CD20/NKp46-CD66b- Tryptase- CD68- MHCII+ CSF1R- DCSIGN- DCLAMP- </t>
-  </si>
-  <si>
-    <t>CD45+ CD3/CD20/NKp46- CD66b- Tryptase- CD68- MHCII+CSF1R- DCSIGN+DC-LAMP-</t>
-  </si>
-  <si>
-    <t>CD45+ CD3/20/NKP46- CD66b- Tryptase- CD68- MHCII-</t>
   </si>
   <si>
     <t>CD45+ CD3- CD20+</t>
@@ -684,9 +443,6 @@
   </si>
   <si>
     <t>CD45+ CD3+ CD8- RORGT+</t>
-  </si>
-  <si>
-    <t>CD45+ CD3+ CD8- FOXP3 +</t>
   </si>
   <si>
     <t>CD45+ CD3+ CD8- FOXP3- RORGT- TBET- GATA3-</t>
@@ -746,13 +502,7 @@
     <t>CD8 T Cells</t>
   </si>
   <si>
-    <t>CD45+ CD3- NKP46- CD20-</t>
-  </si>
-  <si>
     <t>M_on_L</t>
-  </si>
-  <si>
-    <t>CD45+ CD3+ CD8- FoxP3- PD-1+</t>
   </si>
   <si>
     <t>bad_Tcell</t>
@@ -819,6 +569,132 @@
   </si>
   <si>
     <t>Sum</t>
+  </si>
+  <si>
+    <t>CD45+CD3+CD8-FOXP3+</t>
+  </si>
+  <si>
+    <t>CD45+CD3+CD8+PD1+</t>
+  </si>
+  <si>
+    <t>CD45+CD3+CD8+PDL1+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3+CD20+NKp46+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3-CD20-NKp46-</t>
+  </si>
+  <si>
+    <t>CD45+ CD3-CD20-NKp46- CD66b- Tryptase- CD68-</t>
+  </si>
+  <si>
+    <t>CD45+ CD3-CD20-NKp46-CD66b- Tryptase- CD68- MHCII+CSF1R-</t>
+  </si>
+  <si>
+    <t>CD45+ CD3-CD20-NKp46-CD66b- Tryptase- CD68+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3-CD20-NKp46- CD66b- Tryptase-</t>
+  </si>
+  <si>
+    <t>CD45+ CD3+CD20+NKp46+ PDL1+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3+CD20+NKp46- PDL1+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3+CD20+NKp46- Tryptase+ PDL1+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3+CD20+NKp46- CD66b+ PDL1+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3+CD20+NKp46- CD66b- Tryptase- CD68+ CSF1R+ CD163+ PDL1+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3-CD20-NKp46- CD66b- Tryptase- CD68+ CSF1R- CD163+ PDL1+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3-CD20-NKp46- CD66b- Tryptase- CD68+ CSF1R+ CD163- PDL1+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3-20-NKp46- CD66b- Tryptase- CD68+ CD163- CSF1R- PDL1+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3-CD20-NKp46- CD66b- Tryptase- CD68+ PDL1+</t>
+  </si>
+  <si>
+    <t>mature DC PDL1+</t>
+  </si>
+  <si>
+    <t>dual neg DCs PDL1+</t>
+  </si>
+  <si>
+    <t>total DCs PDL1+</t>
+  </si>
+  <si>
+    <t>other myeloid PDL1+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3-CD20-NKp46- Tryptase+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3-CD20-NKp46- CD66b+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3-CD20-NKp46- CD66b- Tryptase- CD68- MHCII+ CSF1R- DCSIGN- DCLAMP+</t>
+  </si>
+  <si>
+    <t>DCSIGN+ DCs PDL1+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD45+ CD3-CD20-NKp46-CD66b- Tryptase- CD68- MHCII+ CSF1R- DCSIGN- DCLAMP- </t>
+  </si>
+  <si>
+    <t>CD45+ CD3-CD20-NKp46- CD66b- Tryptase- CD68- MHCII+CSF1R- DCSIGN+DCLAMP-</t>
+  </si>
+  <si>
+    <t>CD45+ CD3-CD20-NKp46- CD66b- Tryptase- CD68+ CSF1R+ CD163+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3-CD20-NKp46- CD66b- Tryptase- CD68+ CSF1R+ CD163-</t>
+  </si>
+  <si>
+    <t>CD45+ CD3-CD20-NKp46- CD66b- Tryptase- CD68+ CSF1R- CD163-</t>
+  </si>
+  <si>
+    <t>CD45+ CD3-CD20-NKp46- CD66b- Tryptase- CD68- MHCII-</t>
+  </si>
+  <si>
+    <t>CD45+ CD3-CD20-NKp46- CD66b- Tryptase- CD68+ CSF1R- CD163+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3- NKp46- CD20-</t>
+  </si>
+  <si>
+    <t>CD45+ CD3+ CD8- FOXP3- PD1+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3+ CD8- RORGT+PD1+</t>
+  </si>
+  <si>
+    <t>CD45+CD3+CD8-FOXP3+PD1+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3+ CD8- FOXP3- RORGT- TBET- GATA3-PD1+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3+ CD8- TBET+PD1+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3+ CD8- FOXP3- RORGT- GATA3+PD1+</t>
+  </si>
+  <si>
+    <t>CD45+ CD3+ PDL1+</t>
+  </si>
+  <si>
+    <t>CD45+ PD1+</t>
   </si>
 </sst>
 </file>
@@ -6122,8 +5998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6137,13 +6013,13 @@
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>0</v>
@@ -6627,10 +6503,10 @@
         <v>51</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -6791,10 +6667,10 @@
         <v>51</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -7117,10 +6993,10 @@
         <v>51</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>159</v>
+        <v>186</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -7281,10 +7157,10 @@
         <v>51</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -7445,7 +7321,7 @@
         <v>51</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>55</v>
+        <v>184</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9">
@@ -7607,7 +7483,7 @@
         <v>51</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>56</v>
+        <v>187</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10">
@@ -7769,7 +7645,7 @@
         <v>51</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11">
@@ -7931,7 +7807,7 @@
         <v>51</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>58</v>
+        <v>188</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12">
@@ -8093,7 +7969,7 @@
         <v>51</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>59</v>
+        <v>189</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13">
@@ -8255,7 +8131,7 @@
         <v>51</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>60</v>
+        <v>190</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14">
@@ -8417,7 +8293,7 @@
         <v>51</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>61</v>
+        <v>191</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15">
@@ -8579,7 +8455,7 @@
         <v>51</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>62</v>
+        <v>192</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16">
@@ -8741,7 +8617,7 @@
         <v>51</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>63</v>
+        <v>193</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17">
@@ -8903,7 +8779,7 @@
         <v>51</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>64</v>
+        <v>194</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18">
@@ -9065,7 +8941,7 @@
         <v>51</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>65</v>
+        <v>195</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19">
@@ -9227,7 +9103,7 @@
         <v>51</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20">
@@ -9389,7 +9265,7 @@
         <v>51</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>67</v>
+        <v>204</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21">
@@ -9551,7 +9427,7 @@
         <v>51</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>68</v>
+        <v>197</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22">
@@ -9713,7 +9589,7 @@
         <v>51</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>69</v>
+        <v>198</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23">
@@ -9875,7 +9751,7 @@
         <v>51</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>70</v>
+        <v>199</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24">
@@ -10037,7 +9913,7 @@
         <v>51</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>71</v>
+        <v>200</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25">
@@ -10199,7 +10075,7 @@
         <v>51</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26">
@@ -10361,7 +10237,7 @@
         <v>51</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27">
@@ -10523,10 +10399,10 @@
         <v>51</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>131</v>
+        <v>201</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -10687,10 +10563,10 @@
         <v>51</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>128</v>
+        <v>202</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -10851,10 +10727,10 @@
         <v>51</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>126</v>
+        <v>203</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -11015,10 +10891,10 @@
         <v>51</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>162</v>
+        <v>205</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -11179,10 +11055,10 @@
         <v>51</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>163</v>
+        <v>206</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -11343,10 +11219,10 @@
         <v>51</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>122</v>
+        <v>207</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -11507,10 +11383,10 @@
         <v>51</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>120</v>
+        <v>208</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -11671,10 +11547,10 @@
         <v>51</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>118</v>
+        <v>211</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -11835,10 +11711,10 @@
         <v>51</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>115</v>
+        <v>209</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -11999,10 +11875,10 @@
         <v>51</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>164</v>
+        <v>210</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="D37" s="16">
         <v>0</v>
@@ -12160,13 +12036,13 @@
     </row>
     <row r="38" spans="1:54" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>165</v>
+        <v>132</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="D38">
         <v>52</v>
@@ -12324,13 +12200,13 @@
     </row>
     <row r="39" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>166</v>
+        <v>133</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="D39">
         <v>14</v>
@@ -12488,13 +12364,13 @@
     </row>
     <row r="40" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="D40">
         <v>455</v>
@@ -12652,13 +12528,13 @@
     </row>
     <row r="41" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="D41">
         <v>54</v>
@@ -12816,13 +12692,13 @@
     </row>
     <row r="42" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="D42">
         <v>62</v>
@@ -12980,13 +12856,13 @@
     </row>
     <row r="43" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="D43">
         <v>4</v>
@@ -13144,13 +13020,13 @@
     </row>
     <row r="44" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="D44">
         <v>137</v>
@@ -13308,13 +13184,13 @@
     </row>
     <row r="45" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="D45">
         <v>225</v>
@@ -13472,10 +13348,10 @@
     </row>
     <row r="46" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D46">
         <v>25212</v>
@@ -13633,7 +13509,7 @@
     </row>
     <row r="47" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B47" s="22" t="s">
         <v>53</v>
@@ -13795,13 +13671,13 @@
     </row>
     <row r="48" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="C48" s="26" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="D48">
         <v>251</v>
@@ -13959,10 +13835,10 @@
     </row>
     <row r="49" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C49" s="23"/>
       <c r="D49">
@@ -14121,13 +13997,13 @@
     </row>
     <row r="50" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>192</v>
+        <v>213</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>193</v>
+        <v>157</v>
       </c>
       <c r="D50">
         <v>2</v>
@@ -14285,10 +14161,10 @@
     </row>
     <row r="51" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C51" s="23"/>
       <c r="D51">
@@ -14447,13 +14323,13 @@
     </row>
     <row r="52" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>194</v>
+        <v>158</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="D52">
         <v>494</v>
@@ -14611,13 +14487,13 @@
     </row>
     <row r="53" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="D53">
         <v>942</v>
@@ -14775,7 +14651,7 @@
     </row>
     <row r="54" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B54" s="23" t="s">
         <v>54</v>
@@ -14937,12 +14813,14 @@
     </row>
     <row r="55" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="C55" s="24"/>
+        <v>70</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>154</v>
+      </c>
       <c r="D55">
         <v>0</v>
       </c>
@@ -15099,10 +14977,10 @@
     </row>
     <row r="56" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="C56" s="24"/>
       <c r="D56">
@@ -15261,12 +15139,14 @@
     </row>
     <row r="57" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="C57" s="24"/>
+        <v>214</v>
+      </c>
+      <c r="C57" s="24" t="s">
+        <v>79</v>
+      </c>
       <c r="D57">
         <v>0</v>
       </c>
@@ -15423,12 +15303,14 @@
     </row>
     <row r="58" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="C58" s="24"/>
+        <v>215</v>
+      </c>
+      <c r="C58" s="24" t="s">
+        <v>78</v>
+      </c>
       <c r="D58">
         <v>1</v>
       </c>
@@ -15585,12 +15467,14 @@
     </row>
     <row r="59" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="C59" s="24"/>
+        <v>216</v>
+      </c>
+      <c r="C59" s="24" t="s">
+        <v>77</v>
+      </c>
       <c r="D59">
         <v>3</v>
       </c>
@@ -15747,12 +15631,14 @@
     </row>
     <row r="60" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C60" s="24"/>
+        <v>217</v>
+      </c>
+      <c r="C60" s="24" t="s">
+        <v>81</v>
+      </c>
       <c r="D60">
         <v>5</v>
       </c>
@@ -15909,12 +15795,14 @@
     </row>
     <row r="61" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="C61" s="24"/>
+        <v>218</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>80</v>
+      </c>
       <c r="D61">
         <v>1</v>
       </c>
@@ -16071,12 +15959,14 @@
     </row>
     <row r="62" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="C62" s="24"/>
+        <v>180</v>
+      </c>
+      <c r="C62" s="24" t="s">
+        <v>155</v>
+      </c>
       <c r="D62">
         <v>14</v>
       </c>
@@ -16233,12 +16123,14 @@
     </row>
     <row r="63" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="C63" s="24"/>
+        <v>181</v>
+      </c>
+      <c r="C63" s="24" t="s">
+        <v>155</v>
+      </c>
       <c r="D63">
         <v>1</v>
       </c>
@@ -16395,10 +16287,10 @@
     </row>
     <row r="64" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="C64" s="24"/>
       <c r="D64">
@@ -16557,10 +16449,10 @@
     </row>
     <row r="65" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>96</v>
+        <v>219</v>
       </c>
       <c r="C65" s="24"/>
       <c r="D65">
@@ -16719,10 +16611,10 @@
     </row>
     <row r="66" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>97</v>
+        <v>220</v>
       </c>
       <c r="C66" s="24"/>
       <c r="D66">
@@ -16881,10 +16773,10 @@
     </row>
     <row r="67" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="C67" s="24"/>
       <c r="D67">
@@ -17043,10 +16935,10 @@
     </row>
     <row r="68" spans="1:54" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="C68" s="24"/>
       <c r="D68">
@@ -17218,8 +17110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA0A156-810B-1C4B-BF21-7A20FCD76E61}">
   <dimension ref="A1:U70"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:U1"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17231,49 +17123,49 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J1" t="s">
+        <v>167</v>
+      </c>
+      <c r="K1" t="s">
+        <v>168</v>
+      </c>
+      <c r="L1" t="s">
+        <v>169</v>
+      </c>
+      <c r="M1" t="s">
+        <v>170</v>
+      </c>
+      <c r="N1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O1" t="s">
         <v>172</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G1" t="s">
-        <v>200</v>
-      </c>
-      <c r="H1" t="s">
-        <v>201</v>
-      </c>
-      <c r="I1" t="s">
-        <v>202</v>
-      </c>
-      <c r="J1" t="s">
-        <v>203</v>
-      </c>
-      <c r="K1" t="s">
-        <v>204</v>
-      </c>
-      <c r="L1" t="s">
-        <v>205</v>
-      </c>
-      <c r="M1" t="s">
-        <v>206</v>
-      </c>
-      <c r="N1" t="s">
-        <v>207</v>
-      </c>
-      <c r="O1" t="s">
-        <v>208</v>
       </c>
       <c r="P1" t="s">
         <v>38</v>
@@ -17282,13 +17174,13 @@
         <v>39</v>
       </c>
       <c r="R1" t="s">
-        <v>209</v>
+        <v>173</v>
       </c>
       <c r="S1" t="s">
-        <v>210</v>
+        <v>174</v>
       </c>
       <c r="T1" t="s">
-        <v>211</v>
+        <v>175</v>
       </c>
       <c r="U1" t="s">
         <v>50</v>
@@ -17460,10 +17352,10 @@
         <v>51</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="D4">
         <f>Cohort!D4</f>
@@ -17543,10 +17435,10 @@
         <v>51</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="D5">
         <f>Cohort!D5</f>
@@ -17707,10 +17599,10 @@
         <v>51</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>159</v>
+        <v>186</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="D7">
         <f>Cohort!D7</f>
@@ -17790,10 +17682,10 @@
         <v>51</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="D8">
         <f>Cohort!D8</f>
@@ -17873,7 +17765,7 @@
         <v>51</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>55</v>
+        <v>184</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9">
@@ -17954,7 +17846,7 @@
         <v>51</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>56</v>
+        <v>187</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10">
@@ -18035,7 +17927,7 @@
         <v>51</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11">
@@ -18116,7 +18008,7 @@
         <v>51</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>58</v>
+        <v>188</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12">
@@ -18197,7 +18089,7 @@
         <v>51</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>59</v>
+        <v>189</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13">
@@ -18278,7 +18170,7 @@
         <v>51</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>60</v>
+        <v>190</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14">
@@ -18359,7 +18251,7 @@
         <v>51</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>61</v>
+        <v>191</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15">
@@ -18440,7 +18332,7 @@
         <v>51</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>62</v>
+        <v>192</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16">
@@ -18521,7 +18413,7 @@
         <v>51</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>63</v>
+        <v>193</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17">
@@ -18602,7 +18494,7 @@
         <v>51</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>64</v>
+        <v>194</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18">
@@ -18683,7 +18575,7 @@
         <v>51</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>65</v>
+        <v>195</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19">
@@ -18764,7 +18656,7 @@
         <v>51</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20">
@@ -18845,7 +18737,7 @@
         <v>51</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>67</v>
+        <v>204</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21">
@@ -18926,7 +18818,7 @@
         <v>51</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>68</v>
+        <v>197</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22">
@@ -19007,7 +18899,7 @@
         <v>51</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>69</v>
+        <v>198</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23">
@@ -19088,7 +18980,7 @@
         <v>51</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>70</v>
+        <v>199</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24">
@@ -19169,7 +19061,7 @@
         <v>51</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>71</v>
+        <v>200</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25">
@@ -19250,7 +19142,7 @@
         <v>51</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26">
@@ -19331,7 +19223,7 @@
         <v>51</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27">
@@ -19412,10 +19304,10 @@
         <v>51</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>131</v>
+        <v>201</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="D28">
         <f>Cohort!D28</f>
@@ -19495,10 +19387,10 @@
         <v>51</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>128</v>
+        <v>202</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="D29">
         <f>Cohort!D29</f>
@@ -19578,10 +19470,10 @@
         <v>51</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>126</v>
+        <v>203</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="D30">
         <f>Cohort!D30</f>
@@ -19661,10 +19553,10 @@
         <v>51</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>162</v>
+        <v>205</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="D31">
         <f>Cohort!D31</f>
@@ -19744,10 +19636,10 @@
         <v>51</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>163</v>
+        <v>206</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="D32">
         <f>Cohort!D32</f>
@@ -19827,10 +19719,10 @@
         <v>51</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>122</v>
+        <v>207</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D33">
         <f>Cohort!D33</f>
@@ -19910,10 +19802,10 @@
         <v>51</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>120</v>
+        <v>208</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="D34">
         <f>Cohort!D34</f>
@@ -19993,10 +19885,10 @@
         <v>51</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>118</v>
+        <v>211</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="D35">
         <f>Cohort!D35</f>
@@ -20076,10 +19968,10 @@
         <v>51</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>115</v>
+        <v>209</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="D36">
         <f>Cohort!D36</f>
@@ -20159,10 +20051,10 @@
         <v>51</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>164</v>
+        <v>210</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="D37">
         <f>Cohort!D37</f>
@@ -20239,13 +20131,13 @@
     </row>
     <row r="38" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>165</v>
+        <v>132</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="D38">
         <f>Cohort!D38</f>
@@ -20322,13 +20214,13 @@
     </row>
     <row r="39" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>166</v>
+        <v>133</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="D39">
         <f>Cohort!D39</f>
@@ -20405,13 +20297,13 @@
     </row>
     <row r="40" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="D40">
         <f>Cohort!D40</f>
@@ -20488,13 +20380,13 @@
     </row>
     <row r="41" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="D41">
         <f>Cohort!D41</f>
@@ -20571,13 +20463,13 @@
     </row>
     <row r="42" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="D42">
         <f>Cohort!D42</f>
@@ -20654,13 +20546,13 @@
     </row>
     <row r="43" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="D43">
         <f>Cohort!D43</f>
@@ -20737,13 +20629,13 @@
     </row>
     <row r="44" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="D44">
         <f>Cohort!D44</f>
@@ -20820,13 +20712,13 @@
     </row>
     <row r="45" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="D45">
         <f>Cohort!D45</f>
@@ -20903,10 +20795,10 @@
     </row>
     <row r="46" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D46">
         <f>Cohort!D46</f>
@@ -20983,7 +20875,7 @@
     </row>
     <row r="47" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B47" s="22" t="s">
         <v>53</v>
@@ -21064,13 +20956,13 @@
     </row>
     <row r="48" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="C48" s="26" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="D48">
         <f>Cohort!D48</f>
@@ -21147,10 +21039,10 @@
     </row>
     <row r="49" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C49" s="23"/>
       <c r="D49">
@@ -21228,13 +21120,13 @@
     </row>
     <row r="50" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>192</v>
+        <v>213</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>193</v>
+        <v>157</v>
       </c>
       <c r="D50">
         <f>Cohort!D50</f>
@@ -21311,10 +21203,10 @@
     </row>
     <row r="51" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C51" s="23"/>
       <c r="D51">
@@ -21392,13 +21284,13 @@
     </row>
     <row r="52" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>194</v>
+        <v>158</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="D52">
         <f>Cohort!D52</f>
@@ -21475,13 +21367,13 @@
     </row>
     <row r="53" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="D53">
         <f>Cohort!D53</f>
@@ -21558,7 +21450,7 @@
     </row>
     <row r="54" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B54" s="23" t="s">
         <v>54</v>
@@ -21639,12 +21531,14 @@
     </row>
     <row r="55" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="C55" s="24"/>
+        <v>70</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>154</v>
+      </c>
       <c r="D55">
         <f>Cohort!D55</f>
         <v>0</v>
@@ -21720,10 +21614,10 @@
     </row>
     <row r="56" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="C56" s="24"/>
       <c r="D56">
@@ -21801,12 +21695,14 @@
     </row>
     <row r="57" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="C57" s="24"/>
+        <v>214</v>
+      </c>
+      <c r="C57" s="24" t="s">
+        <v>79</v>
+      </c>
       <c r="D57">
         <f>Cohort!D57</f>
         <v>0</v>
@@ -21882,12 +21778,14 @@
     </row>
     <row r="58" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="C58" s="24"/>
+        <v>215</v>
+      </c>
+      <c r="C58" s="24" t="s">
+        <v>78</v>
+      </c>
       <c r="D58">
         <f>Cohort!D58</f>
         <v>1</v>
@@ -21963,12 +21861,14 @@
     </row>
     <row r="59" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="C59" s="24"/>
+        <v>216</v>
+      </c>
+      <c r="C59" s="24" t="s">
+        <v>77</v>
+      </c>
       <c r="D59">
         <f>Cohort!D59</f>
         <v>3</v>
@@ -22044,12 +21944,14 @@
     </row>
     <row r="60" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C60" s="24"/>
+        <v>217</v>
+      </c>
+      <c r="C60" s="24" t="s">
+        <v>81</v>
+      </c>
       <c r="D60">
         <f>Cohort!D60</f>
         <v>5</v>
@@ -22125,12 +22027,14 @@
     </row>
     <row r="61" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="C61" s="24"/>
+        <v>218</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>80</v>
+      </c>
       <c r="D61">
         <f>Cohort!D61</f>
         <v>1</v>
@@ -22206,12 +22110,14 @@
     </row>
     <row r="62" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="C62" s="24"/>
+        <v>180</v>
+      </c>
+      <c r="C62" s="24" t="s">
+        <v>155</v>
+      </c>
       <c r="D62">
         <f>Cohort!D62</f>
         <v>14</v>
@@ -22287,12 +22193,14 @@
     </row>
     <row r="63" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="C63" s="24"/>
+        <v>181</v>
+      </c>
+      <c r="C63" s="24" t="s">
+        <v>155</v>
+      </c>
       <c r="D63">
         <f>Cohort!D63</f>
         <v>1</v>
@@ -22368,10 +22276,10 @@
     </row>
     <row r="64" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="C64" s="24"/>
       <c r="D64">
@@ -22449,10 +22357,10 @@
     </row>
     <row r="65" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>96</v>
+        <v>219</v>
       </c>
       <c r="C65" s="24"/>
       <c r="D65">
@@ -22530,10 +22438,10 @@
     </row>
     <row r="66" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>97</v>
+        <v>220</v>
       </c>
       <c r="C66" s="24"/>
       <c r="D66">
@@ -22611,10 +22519,10 @@
     </row>
     <row r="67" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="C67" s="24"/>
       <c r="D67">
@@ -22692,10 +22600,10 @@
     </row>
     <row r="68" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="C68" s="24"/>
       <c r="D68">
@@ -22786,8 +22694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1728A1F-92C5-2B45-9112-1189A9AD89A0}">
   <dimension ref="A1:U70"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22799,49 +22707,49 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J1" t="s">
+        <v>167</v>
+      </c>
+      <c r="K1" t="s">
+        <v>168</v>
+      </c>
+      <c r="L1" t="s">
+        <v>169</v>
+      </c>
+      <c r="M1" t="s">
+        <v>170</v>
+      </c>
+      <c r="N1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O1" t="s">
         <v>172</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G1" t="s">
-        <v>200</v>
-      </c>
-      <c r="H1" t="s">
-        <v>201</v>
-      </c>
-      <c r="I1" t="s">
-        <v>202</v>
-      </c>
-      <c r="J1" t="s">
-        <v>203</v>
-      </c>
-      <c r="K1" t="s">
-        <v>204</v>
-      </c>
-      <c r="L1" t="s">
-        <v>205</v>
-      </c>
-      <c r="M1" t="s">
-        <v>206</v>
-      </c>
-      <c r="N1" t="s">
-        <v>207</v>
-      </c>
-      <c r="O1" t="s">
-        <v>208</v>
       </c>
       <c r="P1" t="s">
         <v>38</v>
@@ -22850,13 +22758,13 @@
         <v>39</v>
       </c>
       <c r="R1" t="s">
-        <v>209</v>
+        <v>173</v>
       </c>
       <c r="S1" t="s">
-        <v>210</v>
+        <v>174</v>
       </c>
       <c r="T1" t="s">
-        <v>211</v>
+        <v>175</v>
       </c>
       <c r="U1" t="s">
         <v>50</v>
@@ -23028,10 +22936,10 @@
         <v>51</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="D4" t="e">
         <f>Sum!D4 * (Sum!D50 / Sum!D6)</f>
@@ -23111,10 +23019,10 @@
         <v>51</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="D5" t="e">
         <f>Sum!D5 * (Sum!D51 / Sum!D7)</f>
@@ -23275,10 +23183,10 @@
         <v>51</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>159</v>
+        <v>186</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="D7" t="e">
         <f>Sum!D7 * (Sum!D53 / Sum!D9)</f>
@@ -23358,10 +23266,10 @@
         <v>51</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="D8" t="e">
         <f>Sum!D8 * (Sum!D54 / Sum!D10)</f>
@@ -23441,7 +23349,7 @@
         <v>51</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>55</v>
+        <v>184</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" t="e">
@@ -23522,7 +23430,7 @@
         <v>51</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>56</v>
+        <v>187</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" t="e">
@@ -23603,7 +23511,7 @@
         <v>51</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" t="e">
@@ -23684,7 +23592,7 @@
         <v>51</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>58</v>
+        <v>188</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" t="e">
@@ -23765,7 +23673,7 @@
         <v>51</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>59</v>
+        <v>189</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" t="e">
@@ -23846,7 +23754,7 @@
         <v>51</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>60</v>
+        <v>190</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" t="e">
@@ -23927,7 +23835,7 @@
         <v>51</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>61</v>
+        <v>191</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" t="e">
@@ -24008,7 +23916,7 @@
         <v>51</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>62</v>
+        <v>192</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" t="e">
@@ -24089,7 +23997,7 @@
         <v>51</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>63</v>
+        <v>193</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" t="e">
@@ -24170,7 +24078,7 @@
         <v>51</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>64</v>
+        <v>194</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" t="e">
@@ -24251,7 +24159,7 @@
         <v>51</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>65</v>
+        <v>195</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" t="e">
@@ -24332,7 +24240,7 @@
         <v>51</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>66</v>
+        <v>196</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" t="e">
@@ -24413,7 +24321,7 @@
         <v>51</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>67</v>
+        <v>204</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" t="e">
@@ -24494,7 +24402,7 @@
         <v>51</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>68</v>
+        <v>197</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" t="e">
@@ -24575,7 +24483,7 @@
         <v>51</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>69</v>
+        <v>198</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" t="e">
@@ -24656,7 +24564,7 @@
         <v>51</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>70</v>
+        <v>199</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" t="e">
@@ -24737,7 +24645,7 @@
         <v>51</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>71</v>
+        <v>200</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" t="e">
@@ -24818,7 +24726,7 @@
         <v>51</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" t="e">
@@ -24899,7 +24807,7 @@
         <v>51</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" t="e">
@@ -24980,10 +24888,10 @@
         <v>51</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>131</v>
+        <v>201</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="D28" t="e">
         <f>Sum!D28 * (Sum!D74 / Sum!D30)</f>
@@ -25063,10 +24971,10 @@
         <v>51</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>128</v>
+        <v>202</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="D29" t="e">
         <f>Sum!D29 * (Sum!D75 / Sum!D31)</f>
@@ -25146,10 +25054,10 @@
         <v>51</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>126</v>
+        <v>203</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="D30" t="e">
         <f>Sum!D30 * (Sum!D76 / Sum!D32)</f>
@@ -25229,10 +25137,10 @@
         <v>51</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>162</v>
+        <v>205</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="D31" t="e">
         <f>Sum!D31 * (Sum!D77 / Sum!D33)</f>
@@ -25312,10 +25220,10 @@
         <v>51</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>163</v>
+        <v>206</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="D32" t="e">
         <f>Sum!D32 * (Sum!D78 / Sum!D34)</f>
@@ -25395,10 +25303,10 @@
         <v>51</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>122</v>
+        <v>207</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D33" t="e">
         <f>Sum!D33 * (Sum!D79 / Sum!D35)</f>
@@ -25478,10 +25386,10 @@
         <v>51</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>120</v>
+        <v>208</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="D34" t="e">
         <f>Sum!D34 * (Sum!D80 / Sum!D36)</f>
@@ -25561,10 +25469,10 @@
         <v>51</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>118</v>
+        <v>211</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="D35" t="e">
         <f>Sum!D35 * (Sum!D81 / Sum!D37)</f>
@@ -25644,10 +25552,10 @@
         <v>51</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>115</v>
+        <v>209</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="D36">
         <f>Sum!D36 * (Sum!D82 / Sum!D38)</f>
@@ -25727,10 +25635,10 @@
         <v>51</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>164</v>
+        <v>210</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="D37">
         <f>Sum!D37 * (Sum!D83 / Sum!D39)</f>
@@ -25807,13 +25715,13 @@
     </row>
     <row r="38" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>165</v>
+        <v>132</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="D38">
         <f>Sum!D38</f>
@@ -25890,13 +25798,13 @@
     </row>
     <row r="39" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>166</v>
+        <v>133</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="D39">
         <f>Sum!D39</f>
@@ -25973,13 +25881,13 @@
     </row>
     <row r="40" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="D40">
         <f>Sum!D40</f>
@@ -26056,13 +25964,13 @@
     </row>
     <row r="41" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="D41">
         <f>Sum!D41</f>
@@ -26139,13 +26047,13 @@
     </row>
     <row r="42" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="D42">
         <f>Sum!D42</f>
@@ -26222,13 +26130,13 @@
     </row>
     <row r="43" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="D43">
         <f>Sum!D43</f>
@@ -26305,13 +26213,13 @@
     </row>
     <row r="44" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="D44">
         <f>Sum!D44</f>
@@ -26388,13 +26296,13 @@
     </row>
     <row r="45" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="D45">
         <f>Sum!D45</f>
@@ -26471,10 +26379,10 @@
     </row>
     <row r="46" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D46">
         <f>Sum!D46</f>
@@ -26551,7 +26459,7 @@
     </row>
     <row r="47" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B47" s="22" t="s">
         <v>53</v>
@@ -26632,13 +26540,13 @@
     </row>
     <row r="48" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="C48" s="26" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="D48">
         <f>Sum!D48</f>
@@ -26715,10 +26623,10 @@
     </row>
     <row r="49" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C49" s="23"/>
       <c r="D49">
@@ -26796,13 +26704,13 @@
     </row>
     <row r="50" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>192</v>
+        <v>213</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>193</v>
+        <v>157</v>
       </c>
       <c r="D50">
         <f>Sum!D50</f>
@@ -26879,10 +26787,10 @@
     </row>
     <row r="51" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C51" s="23"/>
       <c r="D51">
@@ -26960,13 +26868,13 @@
     </row>
     <row r="52" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>194</v>
+        <v>158</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="D52">
         <f>Sum!D52</f>
@@ -27043,13 +26951,13 @@
     </row>
     <row r="53" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="D53">
         <f>Sum!D53</f>
@@ -27126,7 +27034,7 @@
     </row>
     <row r="54" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B54" s="23" t="s">
         <v>54</v>
@@ -27207,12 +27115,14 @@
     </row>
     <row r="55" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="C55" s="24"/>
+        <v>70</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>154</v>
+      </c>
       <c r="D55">
         <f>Sum!D55</f>
         <v>0</v>
@@ -27288,10 +27198,10 @@
     </row>
     <row r="56" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="C56" s="24"/>
       <c r="D56">
@@ -27369,12 +27279,14 @@
     </row>
     <row r="57" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="C57" s="24"/>
+        <v>214</v>
+      </c>
+      <c r="C57" s="24" t="s">
+        <v>79</v>
+      </c>
       <c r="D57">
         <f>Sum!D57</f>
         <v>0</v>
@@ -27450,12 +27362,14 @@
     </row>
     <row r="58" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="C58" s="24"/>
+        <v>215</v>
+      </c>
+      <c r="C58" s="24" t="s">
+        <v>78</v>
+      </c>
       <c r="D58">
         <f>Sum!D58</f>
         <v>1</v>
@@ -27531,12 +27445,14 @@
     </row>
     <row r="59" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="C59" s="24"/>
+        <v>216</v>
+      </c>
+      <c r="C59" s="24" t="s">
+        <v>77</v>
+      </c>
       <c r="D59">
         <f>Sum!D59</f>
         <v>3</v>
@@ -27612,12 +27528,14 @@
     </row>
     <row r="60" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C60" s="24"/>
+        <v>217</v>
+      </c>
+      <c r="C60" s="24" t="s">
+        <v>81</v>
+      </c>
       <c r="D60">
         <f>Sum!D60</f>
         <v>5</v>
@@ -27693,12 +27611,14 @@
     </row>
     <row r="61" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="C61" s="24"/>
+        <v>218</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>80</v>
+      </c>
       <c r="D61">
         <f>Sum!D61</f>
         <v>1</v>
@@ -27774,12 +27694,14 @@
     </row>
     <row r="62" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="C62" s="24"/>
+        <v>180</v>
+      </c>
+      <c r="C62" s="24" t="s">
+        <v>155</v>
+      </c>
       <c r="D62">
         <f>Sum!D62</f>
         <v>14</v>
@@ -27855,12 +27777,14 @@
     </row>
     <row r="63" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="C63" s="24"/>
+        <v>181</v>
+      </c>
+      <c r="C63" s="24" t="s">
+        <v>155</v>
+      </c>
       <c r="D63">
         <f>Sum!D63</f>
         <v>1</v>
@@ -27936,10 +27860,10 @@
     </row>
     <row r="64" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="C64" s="24"/>
       <c r="D64">
@@ -28017,10 +27941,10 @@
     </row>
     <row r="65" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>96</v>
+        <v>219</v>
       </c>
       <c r="C65" s="24"/>
       <c r="D65">
@@ -28098,10 +28022,10 @@
     </row>
     <row r="66" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>97</v>
+        <v>220</v>
       </c>
       <c r="C66" s="24"/>
       <c r="D66">
@@ -28179,10 +28103,10 @@
     </row>
     <row r="67" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="C67" s="24"/>
       <c r="D67">
@@ -28260,10 +28184,10 @@
     </row>
     <row r="68" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="C68" s="24"/>
       <c r="D68">
@@ -28354,7 +28278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C90890-B489-E041-83A4-B44C708C77C2}">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+    <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
       <selection activeCell="AA23" sqref="AA23"/>
     </sheetView>
   </sheetViews>
@@ -28367,49 +28291,49 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>197</v>
+        <v>161</v>
       </c>
       <c r="E1" t="s">
-        <v>198</v>
+        <v>162</v>
       </c>
       <c r="F1" t="s">
-        <v>199</v>
+        <v>163</v>
       </c>
       <c r="G1" t="s">
-        <v>200</v>
+        <v>164</v>
       </c>
       <c r="H1" t="s">
-        <v>201</v>
+        <v>165</v>
       </c>
       <c r="I1" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="J1" t="s">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="K1" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="L1" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="M1" t="s">
-        <v>206</v>
+        <v>170</v>
       </c>
       <c r="N1" t="s">
-        <v>207</v>
+        <v>171</v>
       </c>
       <c r="O1" t="s">
-        <v>208</v>
+        <v>172</v>
       </c>
       <c r="P1" t="s">
         <v>38</v>
@@ -28418,13 +28342,13 @@
         <v>39</v>
       </c>
       <c r="R1" t="s">
-        <v>209</v>
+        <v>173</v>
       </c>
       <c r="S1" t="s">
-        <v>210</v>
+        <v>174</v>
       </c>
       <c r="T1" t="s">
-        <v>211</v>
+        <v>175</v>
       </c>
       <c r="U1" t="s">
         <v>50</v>
@@ -28432,13 +28356,13 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="45" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="D2">
         <f>Norm!D45/Norm!D$47</f>
@@ -28515,13 +28439,13 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="45" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="D3">
         <f>Norm!D44/Norm!D$47</f>
@@ -28598,13 +28522,13 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="45" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C4" s="51" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="D4">
         <f>Norm!D43/Norm!D$47</f>
@@ -28681,13 +28605,13 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="45" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="D5">
         <f>Norm!D42/Norm!D$47</f>
@@ -28764,13 +28688,13 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="45" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C6" s="53" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="D6">
         <f>Norm!D41/Norm!D$47</f>
@@ -28847,13 +28771,13 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="45" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="D7">
         <f>Norm!D40/Norm!D$47</f>
@@ -28930,13 +28854,13 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="55" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="C8" s="56" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="D8">
         <f>Norm!D39/Norm!D$47</f>
@@ -29013,13 +28937,13 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="55" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="C9" s="57" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="D9">
         <f>Norm!D38/Norm!D$47</f>
@@ -29096,13 +29020,13 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="58" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="C10" s="59" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="D10">
         <f>Norm!D37/Norm!D$47</f>
@@ -29179,13 +29103,13 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="61" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="C11" s="62" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="D11">
         <f>Norm!D36/Norm!D$47</f>
@@ -29262,13 +29186,13 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="61" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="C12" s="63" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="D12" t="e">
         <f>Norm!D35/Norm!D$47</f>
@@ -29345,13 +29269,13 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="61" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="C13" s="64" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="D13" t="e">
         <f>Norm!D34/Norm!D$47</f>
@@ -29428,13 +29352,13 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="61" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="C14" s="65" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D14" t="e">
         <f>Norm!D33/Norm!D$47</f>
@@ -29511,13 +29435,13 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="58" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="C15" s="66" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="D15" t="e">
         <f>Norm!D31/Norm!D$47</f>
@@ -29594,13 +29518,13 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="58" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="C16" s="67" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="D16" t="e">
         <f>Norm!D30/Norm!D$47</f>
@@ -29677,13 +29601,13 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="68" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="C17" s="69" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="D17" t="e">
         <f>Norm!D29/Norm!D$47</f>
@@ -29760,13 +29684,13 @@
     </row>
     <row r="18" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="70" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="C18" s="71" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="D18" s="20" t="e">
         <f>Norm!D28/Norm!D$47</f>
@@ -29843,13 +29767,13 @@
     </row>
     <row r="19" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="75" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
       <c r="B19" s="75" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
       <c r="C19" s="75" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
       <c r="D19" s="76" t="e">
         <f>SUM(D2:D18)</f>
@@ -29926,13 +29850,13 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="B20" s="74" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="C20" s="74" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="D20">
         <f>D6/D5</f>
@@ -30009,13 +29933,13 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B21" s="74" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="C21" s="74" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="D21">
         <f>D8/D3</f>
@@ -30092,13 +30016,13 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>212</v>
+        <v>176</v>
       </c>
       <c r="B22" s="74" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="C22" s="74" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="D22">
         <f>D6/D3</f>
@@ -30175,13 +30099,13 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="B23" s="74" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="C23" s="74" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="D23" t="e">
         <f>D7/SUM(D11:D14)</f>
@@ -30258,13 +30182,13 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="B24" s="74" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="C24" s="74" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="D24" t="e">
         <f>D13/D14</f>
@@ -30341,13 +30265,13 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="B25" s="74" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="C25" s="74" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="D25" t="e">
         <f>D16/D15</f>
@@ -30447,36 +30371,36 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="D1" s="43" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="F1" s="73" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="G1" s="73" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="45" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="D2" s="48">
         <f>E2/SUM(Cohort!E$47:G$47)</f>
@@ -30497,13 +30421,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="45" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="D3" s="48">
         <f>E3/SUM(Cohort!E$47:G$47)</f>
@@ -30524,13 +30448,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="45" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C4" s="51" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="D4" s="48">
         <f>E4/SUM(Cohort!E$47:G$47)</f>
@@ -30551,13 +30475,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="45" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="D5" s="48">
         <f>E5/SUM(Cohort!E$47:G$47)</f>
@@ -30578,13 +30502,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="45" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C6" s="53" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="D6" s="48">
         <f>E6/SUM(Cohort!E$47:G$47)</f>
@@ -30605,13 +30529,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="45" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="D7" s="48">
         <f>E7/SUM(Cohort!E$47:G$47)</f>
@@ -30632,13 +30556,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="55" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="C8" s="56" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="D8" s="48">
         <f>E8/SUM(Cohort!E$47:G$47)</f>
@@ -30659,13 +30583,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="55" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="C9" s="57" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="D9" s="48">
         <f>E9/SUM(Cohort!E$47:G$47)</f>
@@ -30686,13 +30610,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="58" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="C10" s="59" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="D10" s="48">
         <f>E10/SUM(Cohort!E$47:G$47)</f>
@@ -30713,13 +30637,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="61" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="C11" s="62" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="D11" s="48">
         <f>E11/SUM(Cohort!E$47:G$47)</f>
@@ -30740,13 +30664,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="61" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="C12" s="63" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="D12" s="48">
         <f>E12/SUM(Cohort!E$47:G$47)</f>
@@ -30767,13 +30691,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="61" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="C13" s="64" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="D13" s="48">
         <f>E13/SUM(Cohort!E$47:G$47)</f>
@@ -30794,13 +30718,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="61" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="C14" s="65" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D14" s="48">
         <f>E14/SUM(Cohort!E$47:G$47)</f>
@@ -30821,13 +30745,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="58" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="C15" s="66" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="D15" s="48">
         <f>E15/SUM(Cohort!E$47:G$47)</f>
@@ -30848,13 +30772,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="58" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="C16" s="67" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="D16" s="48">
         <f>E16/SUM(Cohort!E$47:G$47)</f>
@@ -30875,13 +30799,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="68" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="C17" s="69" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="D17" s="48">
         <f>E17/SUM(Cohort!E$47:G$47)</f>
@@ -30902,13 +30826,13 @@
     </row>
     <row r="18" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="70" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="C18" s="71" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="D18" s="72">
         <f>E18/SUM(Cohort!E$47:G$47)</f>
@@ -30930,15 +30854,15 @@
     <row r="19" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="34" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="30" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="B21" s="31">
         <f>D6/D5</f>
@@ -30947,7 +30871,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="30" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B22" s="31">
         <f>D8/D3</f>
@@ -30956,7 +30880,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="30" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="B23" s="31">
         <f>D6/D3</f>
@@ -30965,7 +30889,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="B24" s="31">
         <f>D7/SUM(D11:D14)</f>
@@ -30974,7 +30898,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="30" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="B25" s="31">
         <f>D13/D14</f>
@@ -30983,7 +30907,7 @@
     </row>
     <row r="26" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="B26" s="33">
         <f>D16/D15</f>
@@ -30995,32 +30919,32 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="36" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="39" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="40" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="40" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="40" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
@@ -31028,32 +30952,32 @@
     </row>
     <row r="36" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="37" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="38" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="29" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>